<commit_message>
Add HU and Time fix
</commit_message>
<xml_diff>
--- a/testData/LOT.xlsx
+++ b/testData/LOT.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
-    <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
-    <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
+    <sheet name="EU" sheetId="1" r:id="rId1"/>
+    <sheet name="US" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,13 +31,13 @@
     <t>JFK</t>
   </si>
   <si>
-    <t>12.06.2018</t>
-  </si>
-  <si>
-    <t>12.07.2018</t>
-  </si>
-  <si>
     <t>us/en/</t>
+  </si>
+  <si>
+    <t>fr/fr/</t>
+  </si>
+  <si>
+    <t>es/es/</t>
   </si>
 </sst>
 </file>
@@ -355,10 +355,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -367,85 +367,122 @@
     <col min="4" max="4" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D1">
+        <v>20</v>
+      </c>
+      <c r="E1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <v>11</v>
+      </c>
+      <c r="E2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>4</v>
+      <c r="D3">
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>13</v>
+      </c>
+      <c r="E1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>11</v>
+      </c>
+      <c r="E2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>